<commit_message>
Remove bold font inside constraint sheet for r_zsm_3 and cf_signal_12 templates as it does not work with openpyxl when using mixed font inside a same cell.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_cf_signal_12_verification.xlsx
+++ b/prj/src/templates/template_cf_signal_12_verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80DA20A4-93CC-4A74-951C-8CD1C47B5D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB49A6C-932C-4E9D-9680-3B79D9953589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,15 +171,20 @@
     <t>Boolean</t>
   </si>
   <si>
+    <t>Maximum Distance</t>
+  </si>
+  <si>
+    <t>Platform Related</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>CF_SIGNAL_12</t>
+      <t>CF_SIGNAL_12:</t>
     </r>
     <r>
       <rPr>
@@ -188,17 +193,11 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>: Delayed legitimate turnback distance shall ensure the following properties:
+      <t xml:space="preserve"> Delayed legitimate turnback distance shall ensure the following properties:
  - A train shall lock the Signalling approaching zone for sure: therefore it shall be less than the distance between the block limit of the signal and the closest entrance of signalling approach zones of any routes starting from the signal minus at_deshunt_max_dist minus block_laying_uncertainty minus max ([mtc_rollback_dist], [at_rollback_dist], [overshoot_recovery_dist] + [overshoot_recovery_stopping_max_dist]).
  - There shall be no civil infrastructure (switch point, fouling point, derailer, flood gate….) at less than this distance from the block limit of the signal that a train does not lock for sure by shunting the proper blocks.
 0 is a safe value</t>
     </r>
-  </si>
-  <si>
-    <t>Maximum Distance</t>
-  </si>
-  <si>
-    <t>Platform Related</t>
   </si>
 </sst>
 </file>
@@ -327,13 +326,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -347,11 +339,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -363,6 +356,12 @@
     <font>
       <sz val="10"/>
       <name val="Helv"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -535,109 +534,109 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1606,7 +1605,7 @@
   <sheetData>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
@@ -1836,7 +1835,7 @@
         <v>22</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="35" t="s">
         <v>23</v>
@@ -1860,7 +1859,7 @@
         <v>24</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="36" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Fix a problem in IXL APZ computation with depolarization (we need to take the distance upstream the signal and not downstream the IVB limit, as it could be different with depol). Fix a bug in get_dist_downstream function when the other point can be accessed downstream and upstream from the first point and set direction (typically when there is a depol point making a ring).
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_cf_signal_12_verification.xlsx
+++ b/prj/src/templates/template_cf_signal_12_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB49A6C-932C-4E9D-9680-3B79D9953589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FBA2BF-5DA7-4FDF-8ACC-4AD9E41B8EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -162,12 +162,6 @@
     <t>IXL APZ Length</t>
   </si>
   <si>
-    <t>IXL APZ Limit Upstream</t>
-  </si>
-  <si>
-    <t>IXL APZ Limit Downstream</t>
-  </si>
-  <si>
     <t>Boolean</t>
   </si>
   <si>
@@ -198,6 +192,12 @@
  - There shall be no civil infrastructure (switch point, fouling point, derailer, flood gate….) at less than this distance from the block limit of the signal that a train does not lock for sure by shunting the proper blocks.
 0 is a safe value</t>
     </r>
+  </si>
+  <si>
+    <t>Downstream Limit</t>
+  </si>
+  <si>
+    <t>Upstream Limit</t>
   </si>
 </sst>
 </file>
@@ -1436,29 +1436,29 @@
       <selection activeCell="B13" sqref="B13:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="7" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="2" width="16.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="7" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
         <v>11</v>
       </c>
@@ -1467,63 +1467,63 @@
       <c r="E13" s="25"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="29"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="29"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="29"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="29"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="29"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="30"/>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
       <c r="F20" s="32"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1531,7 +1531,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>0</v>
@@ -1545,7 +1545,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1553,7 +1553,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -1561,7 +1561,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -1569,14 +1569,14 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
@@ -1601,11 +1601,11 @@
       <selection activeCell="B4" sqref="B4:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
@@ -1620,7 +1620,7 @@
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -1635,7 +1635,7 @@
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
@@ -1650,7 +1650,7 @@
       <c r="M6" s="34"/>
       <c r="N6" s="34"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -1665,7 +1665,7 @@
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -1680,7 +1680,7 @@
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -1695,7 +1695,7 @@
       <c r="M9" s="34"/>
       <c r="N9" s="34"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -1710,7 +1710,7 @@
       <c r="M10" s="34"/>
       <c r="N10" s="34"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -1725,7 +1725,7 @@
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -1740,7 +1740,7 @@
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -1755,7 +1755,7 @@
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
@@ -1770,7 +1770,7 @@
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
@@ -1803,28 +1803,28 @@
       <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="13" customWidth="1"/>
     <col min="5" max="5" width="14" style="14" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="12" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="12"/>
-    <col min="11" max="11" width="7.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="12"/>
+    <col min="11" max="11" width="7.5546875" style="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="12" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="10.5703125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="10.5546875" style="15" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" style="13" customWidth="1"/>
     <col min="19" max="19" width="39" style="19" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="12"/>
+    <col min="20" max="16384" width="11.44140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>21</v>
       </c>
@@ -1835,19 +1835,19 @@
         <v>22</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="35" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
       <c r="J1" s="41" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
@@ -1859,7 +1859,7 @@
         <v>24</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="36" t="s">
         <v>25</v>
@@ -1871,7 +1871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1961,12 +1961,12 @@
       <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>12</v>
       </c>
@@ -1977,12 +1977,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="42"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>17</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>18</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>19</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
@@ -2036,13 +2036,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete the rich_text argument when loading a template with openpyxl, it was causing fatal errors on other computers. Create a function for the print_log using progress_bar to have a consistent behavior. We needed to add space at the end of the string line so that it erases the previous text that are not erased automatically when using \r carriage return inside the cmd window. Increase the cmd window columns number so that it can display more, so that the carriage returns work properly. Rework the verification of route and overlaps for the names association between DC_SYS and IXL. Update the functions to use the new template of the csv files extracted from the PDF with now only the 4 columns and an added first row to write both the names used by the tool and the name of the info from the PDF. Rework the PDF interpretation with new understanding of the text operations within portable document format. Still to try the functions for the Control Tables PDF on every project.
</commit_message>
<xml_diff>
--- a/prj/src/templates/template_cf_signal_12_verification.xlsx
+++ b/prj/src/templates/template_cf_signal_12_verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naderc\Documents\Python\cbtc_configuration_checking\prj\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F104C8-D45E-4DE8-BC0E-E533A8EF7ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AE6E43-9B6E-48F6-97A5-14D2DD753BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="17" r:id="rId1"/>
@@ -161,24 +161,13 @@
   <si>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CF_SIGNAL_12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
+      <t>CF_SIGNAL_12:</t>
     </r>
     <r>
       <rPr>
@@ -199,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -325,14 +314,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -1358,13 +1339,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="16"/>
+    <col min="1" max="2" width="11.5703125" style="16"/>
     <col min="3" max="3" width="31" style="16" customWidth="1"/>
     <col min="4" max="4" width="51" style="16" customWidth="1"/>
     <col min="5" max="5" width="31" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="11.5546875" style="16"/>
+    <col min="6" max="16384" width="11.5703125" style="16"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1380,12 +1361,12 @@
       <selection activeCell="B4" sqref="B4:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
@@ -1402,7 +1383,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -1417,7 +1398,7 @@
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -1432,7 +1413,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -1447,7 +1428,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -1462,7 +1443,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -1477,7 +1458,7 @@
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -1492,7 +1473,7 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -1507,7 +1488,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -1522,7 +1503,7 @@
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -1537,7 +1518,7 @@
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
@@ -1552,7 +1533,7 @@
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -1585,28 +1566,28 @@
       <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="10" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="10.5546875" style="5" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="10.5703125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" style="3" customWidth="1"/>
     <col min="19" max="19" width="39" style="6" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="2"/>
+    <col min="20" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
@@ -1653,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1690,7 +1671,7 @@
       <c r="R2" s="21"/>
       <c r="S2" s="21"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D3" s="15"/>
       <c r="E3" s="14"/>
     </row>
@@ -1747,13 +1728,13 @@
       <selection pane="bottomLeft" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="37.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
@@ -1764,12 +1745,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
@@ -1778,7 +1759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -1787,7 +1768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1796,7 +1777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -1805,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
@@ -1814,7 +1795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
@@ -1823,7 +1804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>

</xml_diff>